<commit_message>
added features for base project.
</commit_message>
<xml_diff>
--- a/mnt/data/input.xlsx
+++ b/mnt/data/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\OneDrive\Documents\archive\tesis_2023\src\MLSA-pipeline\mnt\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/archive/tesis_2023/src/MLSA-pipeline/mnt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB11AB2-AD0A-4D91-9D16-99DD47847BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9BB11AB2-AD0A-4D91-9D16-99DD47847BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65ADC5BE-26B7-4A59-A1C9-CD99DA945D5E}"/>
   <bookViews>
-    <workbookView xWindow="35535" yWindow="4125" windowWidth="19170" windowHeight="10065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,8 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -439,64 +438,70 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed basic funcitonality of pipeline
</commit_message>
<xml_diff>
--- a/mnt/data/input.xlsx
+++ b/mnt/data/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/archive/tesis_2023/src/MLSA-pipeline/mnt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9BB11AB2-AD0A-4D91-9D16-99DD47847BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65ADC5BE-26B7-4A59-A1C9-CD99DA945D5E}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{9BB11AB2-AD0A-4D91-9D16-99DD47847BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E5F156D-F5F2-4EF8-A510-758739DC7C59}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Organism</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>S_cerevisiae_recA.fasta</t>
+  </si>
+  <si>
+    <t>Saccharomyceo cochise</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,7 +508,22 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>